<commit_message>
Atualização dos intervalos de umidade
</commit_message>
<xml_diff>
--- a/Documentos/Intervalos ArqComp..xlsx
+++ b/Documentos/Intervalos ArqComp..xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinys\OneDrive\Área de Trabalho\BandTec\Git Hub\Projeto Git\Amonimous\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Amonimous\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03BC7FA-E8E7-4EA3-A690-801B0A5C19B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>TEMPERATURA</t>
   </si>
@@ -53,27 +52,6 @@
     <t>Tolerável</t>
   </si>
   <si>
-    <t>Alerta</t>
-  </si>
-  <si>
-    <t>Minimo</t>
-  </si>
-  <si>
-    <t>1°Q</t>
-  </si>
-  <si>
-    <t>média</t>
-  </si>
-  <si>
-    <t>mediana</t>
-  </si>
-  <si>
-    <t>3°Q</t>
-  </si>
-  <si>
-    <t>Máximo</t>
-  </si>
-  <si>
     <t>Atenção</t>
   </si>
   <si>
@@ -81,13 +59,82 @@
   </si>
   <si>
     <t>QUARTIS UMIDADE</t>
+  </si>
+  <si>
+    <t>Nível</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>Porcentagem de medição</t>
+  </si>
+  <si>
+    <t>Função</t>
+  </si>
+  <si>
+    <t>f(j) = T * j = T * 1,00</t>
+  </si>
+  <si>
+    <t>f(i) = T * i = T * 0,96</t>
+  </si>
+  <si>
+    <t>f(h) = T * h =  T * 0,91</t>
+  </si>
+  <si>
+    <t>f(g) = T * g =  T * 0,87</t>
+  </si>
+  <si>
+    <t>f(f) = T * f =  T * 0,82</t>
+  </si>
+  <si>
+    <t>f(e) = T * e =  T * 0,78</t>
+  </si>
+  <si>
+    <t>f(d) = T * d =  T * 0,74</t>
+  </si>
+  <si>
+    <t>f(c) = T * c =  T * 0,69</t>
+  </si>
+  <si>
+    <t>f(b) = T * b =  T * 0,65</t>
+  </si>
+  <si>
+    <t>f(a) = T * a =  T * 0,60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -116,8 +163,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -180,24 +234,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF3B3B"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA9D18E"/>
-        <bgColor rgb="FF92D050"/>
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -260,54 +302,273 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -691,11 +952,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,236 +966,372 @@
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" customWidth="1"/>
+    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
+    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="2"/>
-      <c r="E2" s="1" t="s">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="C2" s="26"/>
+      <c r="E2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="H2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="I2" s="26"/>
+      <c r="K2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="18"/>
+      <c r="N2" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="34"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="4">
+        <v>20</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="4">
+        <v>20</v>
+      </c>
+      <c r="N3" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" s="30">
+        <v>1</v>
+      </c>
+      <c r="P3" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="36"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6">
+        <f>C3+7.7</f>
+        <v>11.7</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="10">
+        <f>_xlfn.QUARTILE.EXC(C3:C10,1)</f>
+        <v>13.625</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="8">
+        <f>I3+9.85</f>
+        <v>29.85</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="8">
+        <f>_xlfn.QUARTILE.EXC(I3:I7,1)</f>
+        <v>24.925000000000001</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" s="31">
+        <f>O3-0.044</f>
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="P4" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="36"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="10">
+        <f>C4+7.7</f>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <f>MEDIAN(C3:C10)</f>
+        <v>25</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="12">
+        <f t="shared" ref="I5:I6" si="0">I4+9.85</f>
+        <v>39.700000000000003</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="12">
+        <f>MEDIAN(I3:I7)</f>
+        <v>39.700000000000003</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="31">
+        <f t="shared" ref="O5:O11" si="1">O4-0.044</f>
+        <v>0.91199999999999992</v>
+      </c>
+      <c r="P5" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="36"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>23</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="12">
+        <f>_xlfn.QUARTILE.EXC(C3:C10,3)</f>
+        <v>30.4375</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="0"/>
+        <v>49.550000000000004</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" s="14">
+        <f>_xlfn.QUARTILE.EXC(I3:I7,3)</f>
+        <v>54.475000000000001</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="O6" s="31">
+        <f t="shared" si="1"/>
+        <v>0.86799999999999988</v>
+      </c>
+      <c r="P6" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q6" s="36"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>27</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="16">
+        <v>32</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="16">
+        <v>59.4</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="16">
+        <v>59.4</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="31">
+        <f t="shared" si="1"/>
+        <v>0.82399999999999984</v>
+      </c>
+      <c r="P7" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="36"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12">
+        <v>29.5</v>
+      </c>
+      <c r="N8" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="N2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E3" s="3" t="s">
+      <c r="O8" s="31">
+        <f t="shared" si="1"/>
+        <v>0.7799999999999998</v>
+      </c>
+      <c r="P8" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="36"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="14">
+        <f>(C8+C10)/2</f>
+        <v>30.75</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="O9" s="31">
+        <f t="shared" si="1"/>
+        <v>0.73599999999999977</v>
+      </c>
+      <c r="P9" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="36"/>
+    </row>
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="4">
-        <v>4</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L3" s="4">
-        <v>4</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="8">
-        <f>F3+7.7</f>
-        <v>11.7</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="10">
-        <f>I3+14.85</f>
-        <v>14.85</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="12">
-        <f>_xlfn.QUARTILE.EXC(F3:F10,1)</f>
-        <v>13.625</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O4" s="10">
-        <f>_xlfn.QUARTILE.EXC(I3:I7,1)</f>
-        <v>7.4249999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="12">
-        <f>F4+7.7</f>
-        <v>19.399999999999999</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="14">
-        <f>I4+14.85</f>
-        <v>29.7</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="L5" s="6">
-        <f>MEDIAN(F3:F10)</f>
-        <v>25</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="O5" s="14">
-        <f>MEDIAN(I3:I7)</f>
-        <v>29.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="6">
-        <v>23</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" s="16">
-        <f>I5+14.85</f>
-        <v>44.55</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="14">
-        <f>_xlfn.QUARTILE.EXC(F3:F10,3)</f>
-        <v>30.4375</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="O6" s="16">
-        <f>_xlfn.QUARTILE.EXC(I3:I7,3)</f>
-        <v>51.974999999999994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="10">
-        <v>27</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" s="18">
-        <v>59.4</v>
-      </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L7" s="18">
+      <c r="C10" s="16">
         <v>32</v>
       </c>
-      <c r="N7" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="O7" s="18">
-        <v>59.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E8" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="14">
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="16">
-        <f>(F8+F10)/2</f>
-        <v>30.75</v>
-      </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="18">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="N10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="O10" s="31">
+        <f t="shared" si="1"/>
+        <v>0.69199999999999973</v>
+      </c>
+      <c r="P10" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10" s="36"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="31">
+        <f t="shared" si="1"/>
+        <v>0.64799999999999969</v>
+      </c>
+      <c r="P11" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="36"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
-        <v>12</v>
-      </c>
+      <c r="O12" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="P12" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="38"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="27"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="27"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="15">
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>